<commit_message>
add final edited report in pdf format
</commit_message>
<xml_diff>
--- a/survey/excel/sf4.xlsx
+++ b/survey/excel/sf4.xlsx
@@ -2571,11 +2571,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="147102336"/>
-        <c:axId val="147104128"/>
+        <c:axId val="125867520"/>
+        <c:axId val="125869056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="147102336"/>
+        <c:axId val="125867520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2584,7 +2584,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147104128"/>
+        <c:crossAx val="125869056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2592,7 +2592,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147104128"/>
+        <c:axId val="125869056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2608,7 +2608,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="147102336"/>
+        <c:crossAx val="125867520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4121,11 +4121,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="147282560"/>
-        <c:axId val="147296640"/>
+        <c:axId val="125900288"/>
+        <c:axId val="125901824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="147282560"/>
+        <c:axId val="125900288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4134,7 +4134,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147296640"/>
+        <c:crossAx val="125901824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4142,7 +4142,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147296640"/>
+        <c:axId val="125901824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4153,7 +4153,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147282560"/>
+        <c:crossAx val="125900288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4313,11 +4313,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="147306752"/>
-        <c:axId val="147316736"/>
+        <c:axId val="125922688"/>
+        <c:axId val="125944960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="147306752"/>
+        <c:axId val="125922688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4327,7 +4327,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147316736"/>
+        <c:crossAx val="125944960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4335,7 +4335,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147316736"/>
+        <c:axId val="125944960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4346,7 +4346,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147306752"/>
+        <c:crossAx val="125922688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4505,11 +4505,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="150282240"/>
-        <c:axId val="150283776"/>
+        <c:axId val="125969536"/>
+        <c:axId val="125971072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="150282240"/>
+        <c:axId val="125969536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4519,7 +4519,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150283776"/>
+        <c:crossAx val="125971072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4527,7 +4527,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150283776"/>
+        <c:axId val="125971072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4538,7 +4538,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150282240"/>
+        <c:crossAx val="125969536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4701,11 +4701,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="150312832"/>
-        <c:axId val="150314368"/>
+        <c:axId val="126016128"/>
+        <c:axId val="126091648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="150312832"/>
+        <c:axId val="126016128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4714,7 +4714,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150314368"/>
+        <c:crossAx val="126091648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4722,7 +4722,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150314368"/>
+        <c:axId val="126091648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4733,7 +4733,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150312832"/>
+        <c:crossAx val="126016128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4880,11 +4880,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="150337792"/>
-        <c:axId val="150429696"/>
+        <c:axId val="126104320"/>
+        <c:axId val="126105856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="150337792"/>
+        <c:axId val="126104320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4894,7 +4894,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150429696"/>
+        <c:crossAx val="126105856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4902,7 +4902,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150429696"/>
+        <c:axId val="126105856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4913,7 +4913,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150337792"/>
+        <c:crossAx val="126104320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5345,11 +5345,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="42735104"/>
-        <c:axId val="42658816"/>
+        <c:axId val="126138240"/>
+        <c:axId val="145481728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42735104"/>
+        <c:axId val="126138240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -5379,12 +5379,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42658816"/>
+        <c:crossAx val="145481728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42658816"/>
+        <c:axId val="145481728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5414,7 +5414,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42735104"/>
+        <c:crossAx val="126138240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5846,11 +5846,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="44563456"/>
-        <c:axId val="44334464"/>
+        <c:axId val="145551360"/>
+        <c:axId val="145553280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44563456"/>
+        <c:axId val="145551360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -5880,12 +5880,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44334464"/>
+        <c:crossAx val="145553280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44334464"/>
+        <c:axId val="145553280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -5916,7 +5916,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44563456"/>
+        <c:crossAx val="145551360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6497,7 +6497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="T110" sqref="T110"/>
     </sheetView>
   </sheetViews>
@@ -8709,7 +8709,7 @@
         <v>2</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34:F65" si="8">SUM(B34:E34)</f>
+        <f t="shared" ref="F34:F55" si="8">SUM(B34:E34)</f>
         <v>4</v>
       </c>
       <c r="G34">

</xml_diff>